<commit_message>
Updates Cha Cha and Leo Leo files
</commit_message>
<xml_diff>
--- a/Cha Cha - VCLFO/BOM.xlsx
+++ b/Cha Cha - VCLFO/BOM.xlsx
@@ -8,7 +8,7 @@
     <sheet state="visible" name="Tayda Auto Order - Export as CS" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'CONTROL BOARD'!$A$1:$E$18</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'CONTROL BOARD'!$A$1:$E$19</definedName>
     <definedName hidden="1" localSheetId="1" name="_xlnm._FilterDatabase">'MAIN BOARD'!$A$1:$E$24</definedName>
   </definedNames>
   <calcPr/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,18 @@
   </si>
   <si>
     <t>https://www.taydaelectronics.com/8-pin-dip-ic-socket-machine-tooled.html</t>
+  </si>
+  <si>
+    <t>Knobs</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Knob DAVIES 1900H CLONE Cream</t>
+  </si>
+  <si>
+    <t>https://www.taydaelectronics.com/knob-davies-1900h-clone-cream.html</t>
   </si>
   <si>
     <t>Notes</t>
@@ -485,6 +497,9 @@
   </si>
   <si>
     <t>A-1317</t>
+  </si>
+  <si>
+    <t>A-4560</t>
   </si>
 </sst>
 </file>
@@ -1162,10 +1177,27 @@
         <v>61</v>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="$A$1:$E$18">
-    <sortState ref="A1:E18">
-      <sortCondition ref="A1:A18"/>
+  <autoFilter ref="$A$1:$E$19">
+    <sortState ref="A1:E19">
+      <sortCondition ref="A1:A19"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -1186,11 +1218,12 @@
     <hyperlink r:id="rId15" ref="E16"/>
     <hyperlink r:id="rId16" ref="E17"/>
     <hyperlink r:id="rId17" ref="E18"/>
+    <hyperlink r:id="rId18" ref="E19"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
   <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
-  <drawing r:id="rId18"/>
+  <drawing r:id="rId19"/>
 </worksheet>
 </file>
 
@@ -1226,15 +1259,15 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>15</v>
@@ -1251,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>7</v>
@@ -1265,70 +1298,70 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D4" s="13">
         <v>2.0</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D5" s="13">
         <v>2.0</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="D6" s="13">
         <v>2.0</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="D7" s="13">
         <v>1.0</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8">
@@ -1336,7 +1369,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>40</v>
@@ -1350,19 +1383,19 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D9" s="13">
         <v>1.0</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10">
@@ -1370,7 +1403,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>19</v>
@@ -1387,7 +1420,7 @@
         <v>32</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>19</v>
@@ -1404,7 +1437,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>19</v>
@@ -1421,7 +1454,7 @@
         <v>470.0</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>19</v>
@@ -1435,10 +1468,10 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>19</v>
@@ -1455,7 +1488,7 @@
         <v>220.0</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>19</v>
@@ -1469,10 +1502,10 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>19</v>
@@ -1489,7 +1522,7 @@
         <v>10.0</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>19</v>
@@ -1503,10 +1536,10 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>19</v>
@@ -1520,10 +1553,10 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>19</v>
@@ -1540,84 +1573,84 @@
         <v>9</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D20" s="13">
         <v>1.0</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D21" s="13">
         <v>1.0</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D22" s="13">
         <v>1.0</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="7" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D23" s="7">
         <v>2.0</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="15" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D24" s="15">
         <v>2.0</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1666,15 +1699,15 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="17" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="17" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B2" s="7">
         <v>10.0</v>
@@ -1682,7 +1715,7 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="B3" s="7">
         <v>20.0</v>
@@ -1690,7 +1723,7 @@
     </row>
     <row r="4">
       <c r="A4" s="17" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B4" s="7">
         <v>10.0</v>
@@ -1698,7 +1731,7 @@
     </row>
     <row r="5">
       <c r="A5" s="17" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B5" s="7">
         <v>10.0</v>
@@ -1706,7 +1739,7 @@
     </row>
     <row r="6">
       <c r="A6" s="17" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B6" s="7">
         <v>10.0</v>
@@ -1714,7 +1747,7 @@
     </row>
     <row r="7">
       <c r="A7" s="17" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="B7" s="7">
         <v>10.0</v>
@@ -1722,7 +1755,7 @@
     </row>
     <row r="8">
       <c r="A8" s="17" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="B8" s="7">
         <v>10.0</v>
@@ -1730,7 +1763,7 @@
     </row>
     <row r="9">
       <c r="A9" s="17" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="B9" s="7">
         <v>10.0</v>
@@ -1738,7 +1771,7 @@
     </row>
     <row r="10">
       <c r="A10" s="17" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B10" s="7">
         <v>10.0</v>
@@ -1746,7 +1779,7 @@
     </row>
     <row r="11">
       <c r="A11" s="17" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B11" s="7">
         <v>10.0</v>
@@ -1754,7 +1787,7 @@
     </row>
     <row r="12">
       <c r="A12" s="17" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B12" s="7">
         <v>10.0</v>
@@ -1762,7 +1795,7 @@
     </row>
     <row r="13">
       <c r="A13" s="17" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="B13" s="7">
         <v>10.0</v>
@@ -1770,7 +1803,7 @@
     </row>
     <row r="14">
       <c r="A14" s="17" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B14" s="7">
         <v>10.0</v>
@@ -1778,7 +1811,7 @@
     </row>
     <row r="15">
       <c r="A15" s="17" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="B15" s="7">
         <v>10.0</v>
@@ -1786,7 +1819,7 @@
     </row>
     <row r="16">
       <c r="A16" s="17" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B16" s="7">
         <v>10.0</v>
@@ -1794,7 +1827,7 @@
     </row>
     <row r="17">
       <c r="A17" s="17" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="B17" s="7">
         <v>2.0</v>
@@ -1802,7 +1835,7 @@
     </row>
     <row r="18">
       <c r="A18" s="17" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="B18" s="7">
         <v>2.0</v>
@@ -1810,7 +1843,7 @@
     </row>
     <row r="19">
       <c r="A19" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="B19" s="7">
         <v>2.0</v>
@@ -1818,7 +1851,7 @@
     </row>
     <row r="20">
       <c r="A20" s="17" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="B20" s="7">
         <v>5.0</v>
@@ -1826,7 +1859,7 @@
     </row>
     <row r="21">
       <c r="A21" s="17" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="B21" s="7">
         <v>1.0</v>
@@ -1834,7 +1867,7 @@
     </row>
     <row r="22">
       <c r="A22" s="17" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B22" s="7">
         <v>1.0</v>
@@ -1842,7 +1875,7 @@
     </row>
     <row r="23">
       <c r="A23" s="17" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="B23" s="7">
         <v>6.0</v>
@@ -1850,7 +1883,7 @@
     </row>
     <row r="24">
       <c r="A24" s="17" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="B24" s="7">
         <v>1.0</v>
@@ -1858,7 +1891,7 @@
     </row>
     <row r="25">
       <c r="A25" s="17" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="B25" s="7">
         <v>1.0</v>
@@ -1866,7 +1899,7 @@
     </row>
     <row r="26">
       <c r="A26" s="17" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="B26" s="7">
         <v>2.0</v>
@@ -1874,7 +1907,7 @@
     </row>
     <row r="27">
       <c r="A27" s="17" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B27" s="7">
         <v>2.0</v>
@@ -1882,7 +1915,7 @@
     </row>
     <row r="28">
       <c r="A28" s="17" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="B28" s="7">
         <v>2.0</v>
@@ -1890,7 +1923,7 @@
     </row>
     <row r="29">
       <c r="A29" s="17" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B29" s="7">
         <v>1.0</v>
@@ -1898,7 +1931,7 @@
     </row>
     <row r="30">
       <c r="A30" s="17" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="B30" s="7">
         <v>1.0</v>
@@ -1906,7 +1939,7 @@
     </row>
     <row r="31">
       <c r="A31" s="17" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="B31" s="7">
         <v>1.0</v>
@@ -1914,7 +1947,7 @@
     </row>
     <row r="32">
       <c r="A32" s="17" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="B32" s="7">
         <v>1.0</v>
@@ -1922,7 +1955,7 @@
     </row>
     <row r="33">
       <c r="A33" s="17" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="B33" s="7">
         <v>1.0</v>
@@ -1930,7 +1963,7 @@
     </row>
     <row r="34">
       <c r="A34" s="17" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="B34" s="7">
         <v>2.0</v>
@@ -1938,14 +1971,19 @@
     </row>
     <row r="35">
       <c r="A35" s="17" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="B35" s="7">
         <v>2.0</v>
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="7"/>
+      <c r="A36" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="B36" s="7">
+        <v>2.0</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" s="7"/>

</xml_diff>